<commit_message>
Changes made in the project report
</commit_message>
<xml_diff>
--- a/global_data.xlsx
+++ b/global_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheru\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UDACITY\Data Analyst Foundations NanoDegree\PROJECTS\Explore Weather Trends\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3150,16 +3150,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3487,7 +3487,7 @@
   <dimension ref="A1:C267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C267" activeCellId="1" sqref="A1:A267 C1:C267"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>